<commit_message>
update selenium find tags
</commit_message>
<xml_diff>
--- a/data/scorecards/scorecard_0.xlsx
+++ b/data/scorecards/scorecard_0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="65">
   <si>
     <t>1</t>
   </si>
@@ -115,142 +115,100 @@
     <t>Penalties</t>
   </si>
   <si>
-    <t>483</t>
+    <t>348</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>593</t>
+  </si>
+  <si>
+    <t>318</t>
+  </si>
+  <si>
+    <t>494</t>
+  </si>
+  <si>
+    <t>3026</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>634</t>
   </si>
   <si>
     <t>1W</t>
   </si>
   <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>163</t>
+    <t>337</t>
+  </si>
+  <si>
+    <t>3W</t>
+  </si>
+  <si>
+    <t>Pw</t>
+  </si>
+  <si>
+    <t>331</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>5W</t>
   </si>
   <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>3W</t>
-  </si>
-  <si>
-    <t>476</t>
-  </si>
-  <si>
     <t>304</t>
   </si>
   <si>
-    <t>312</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>7i</t>
-  </si>
-  <si>
-    <t>341</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>2879</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>86%</t>
-  </si>
-  <si>
-    <t>13%</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>133</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Pw</t>
-  </si>
-  <si>
-    <t>310</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>437</t>
-  </si>
-  <si>
-    <t>278</t>
-  </si>
-  <si>
-    <t>317</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>6i</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>379</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>2764</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>43%</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>5644</t>
+    <t>267</t>
+  </si>
+  <si>
+    <t>8i</t>
+  </si>
+  <si>
+    <t>395</t>
+  </si>
+  <si>
+    <t>362</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>2913</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>29%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>5939</t>
   </si>
   <si>
     <t>72</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>64%</t>
-  </si>
-  <si>
-    <t>35</t>
   </si>
 </sst>
 </file>
@@ -687,64 +645,64 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" t="s">
         <v>54</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
         <v>56</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="V2" t="s">
         <v>63</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -752,67 +710,67 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="M3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" t="s">
-        <v>0</v>
-      </c>
       <c r="U3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -820,46 +778,46 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
         <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" t="s">
-        <v>4</v>
       </c>
       <c r="P4" t="s">
         <v>3</v>
@@ -868,87 +826,60 @@
         <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S4" t="s">
         <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="V4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="M5" t="s">
         <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" t="s">
-        <v>2</v>
       </c>
       <c r="N5" t="s">
         <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P5" t="s">
         <v>6</v>
       </c>
       <c r="Q5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R5" t="s">
         <v>5</v>
       </c>
       <c r="S5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="U5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="V5" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -956,67 +887,67 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="S6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
+      <c r="U6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P6" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" t="s">
-        <v>69</v>
-      </c>
-      <c r="U6" t="s">
-        <v>11</v>
-      </c>
       <c r="V6" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1024,67 +955,67 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="N7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
-        <v>0</v>
-      </c>
       <c r="S7" t="s">
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="V7" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1098,89 +1029,83 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" t="s">
-        <v>34</v>
-      </c>
       <c r="M8" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="N8" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="O8" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="Q8" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="R8" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="T8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="U8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K9" t="s">
-        <v>52</v>
-      </c>
       <c r="U9" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="V9" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K10" t="s">
-        <v>53</v>
-      </c>
       <c r="U10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="V10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1188,67 +1113,67 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="J11" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="L11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M11" t="s">
         <v>1</v>
       </c>
       <c r="N11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
         <v>1</v>
       </c>
-      <c r="O11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" t="s">
-        <v>2</v>
-      </c>
       <c r="S11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="V11" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -1256,64 +1181,64 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="L12" t="s">
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="O12" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V12" t="s">
         <v>2</v>
@@ -1324,67 +1249,67 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I13" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="L13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O13" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="P13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S13" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U13" t="s">
         <v>0</v>
       </c>
       <c r="V13" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>